<commit_message>
Added EntityAIAntGoTo and added ants to Ants.xlsx
</commit_message>
<xml_diff>
--- a/other/Ants2.xlsx
+++ b/other/Ants2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="13860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
   <si>
     <t>Species</t>
   </si>
@@ -201,9 +201,6 @@
     <t>Damages nearby entities</t>
   </si>
   <si>
-    <t>Mines neaby blocks</t>
-  </si>
-  <si>
     <t>Picks up all dropped items</t>
   </si>
   <si>
@@ -214,6 +211,39 @@
   </si>
   <si>
     <t>Produces formic acid</t>
+  </si>
+  <si>
+    <t>5th Stage</t>
+  </si>
+  <si>
+    <t>Ferrum (ext Dredger)</t>
+  </si>
+  <si>
+    <t>Mines neaby blocks with stone harvest level</t>
+  </si>
+  <si>
+    <t>Myrmidon (ext. hostile)</t>
+  </si>
+  <si>
+    <t>Hostile + Canticum</t>
+  </si>
+  <si>
+    <t>Dredger + Canticum</t>
+  </si>
+  <si>
+    <t>Mines blocks with iron harvest level</t>
+  </si>
+  <si>
+    <t>Tameable ant that fights for you</t>
+  </si>
+  <si>
+    <t>Canticum</t>
+  </si>
+  <si>
+    <t>FOUND IN DIMENSION</t>
+  </si>
+  <si>
+    <t>Dimension</t>
   </si>
 </sst>
 </file>
@@ -226,6 +256,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -645,19 +676,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1044,7 +1076,7 @@
         <v>51</v>
       </c>
       <c r="I21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1151,16 +1183,16 @@
         <v>7</v>
       </c>
       <c r="F25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" t="s">
         <v>20</v>
       </c>
       <c r="I25" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1189,7 +1221,7 @@
         <v>54</v>
       </c>
       <c r="I26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1218,7 +1250,7 @@
         <v>55</v>
       </c>
       <c r="I27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1247,7 +1279,60 @@
         <v>56</v>
       </c>
       <c r="I28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="2" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31" t="s">
+        <v>69</v>
+      </c>
+      <c r="I31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32" t="s">
+        <v>68</v>
+      </c>
+      <c r="I32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added breeding chamber recipes and achievements
</commit_message>
<xml_diff>
--- a/other/Ants2.xlsx
+++ b/other/Ants2.xlsx
@@ -204,9 +204,6 @@
     <t>Picks up all dropped items</t>
   </si>
   <si>
-    <t>Grows neaby crops</t>
-  </si>
-  <si>
     <t>Tends to animals</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>Dimension</t>
+  </si>
+  <si>
+    <t>Grows crops</t>
   </si>
 </sst>
 </file>
@@ -678,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1192,7 +1192,7 @@
         <v>20</v>
       </c>
       <c r="I25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1250,7 +1250,7 @@
         <v>55</v>
       </c>
       <c r="I27" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1279,60 +1279,60 @@
         <v>56</v>
       </c>
       <c r="I28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H31" t="s">
+        <v>68</v>
+      </c>
+      <c r="I31" t="s">
         <v>69</v>
-      </c>
-      <c r="I31" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" t="s">
         <v>67</v>
       </c>
-      <c r="H32" t="s">
-        <v>68</v>
-      </c>
       <c r="I32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
         <v>72</v>
-      </c>
-      <c r="B33" t="b">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33">
-        <v>10</v>
-      </c>
-      <c r="E33" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" t="b">
-        <v>1</v>
-      </c>
-      <c r="G33" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>